<commit_message>
Hiển thị danh sách tin
</commit_message>
<xml_diff>
--- a/me-docs/33.Xay-dung-Frontend-hien-thi-tin-tuc-RSS.xlsx
+++ b/me-docs/33.Xay-dung-Frontend-hien-thi-tin-tuc-RSS.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\proj_news\me-docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF5C3A0-7278-4A21-AF06-327553BDEF20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{579B65B1-03DF-4822-8701-ED8EDE85BDE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Đọc RSS VNExpress and TuoiTre" sheetId="1" r:id="rId1"/>
+    <sheet name="Hiển thị danh sách tin" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>routes\web.php</t>
   </si>
@@ -39,9 +40,6 @@
     <t>app\Helpers\Feed.php</t>
   </si>
   <si>
-    <t>preg_match('/src="(.+)"/i', $value['description'], $tmp1);</t>
-  </si>
-  <si>
     <t>preg_match('/' . $pattern . '/', $value['description'], $tmp2);</t>
   </si>
   <si>
@@ -49,6 +47,21 @@
   </si>
   <si>
     <t>app\Http\Controllers\News\RssController.php</t>
+  </si>
+  <si>
+    <t>preg_match('/src="(.+)".*&gt;&lt;\/a&gt;/i', $value['description'], $tmp1);</t>
+  </si>
+  <si>
+    <t>resources\views\news\pages\rss\index.blade.php</t>
+  </si>
+  <si>
+    <t>resources\views\news\pages\rss\child-index\list.blade.php</t>
+  </si>
+  <si>
+    <t>Check browser</t>
+  </si>
+  <si>
+    <t>Result</t>
   </si>
 </sst>
 </file>
@@ -337,94 +350,6 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>275124</xdr:colOff>
-      <xdr:row>101</xdr:row>
-      <xdr:rowOff>142238</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3FDDFAD-DA86-E66A-FF63-56CD0DAA827A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="609600" y="14287500"/>
-          <a:ext cx="8809524" cy="5095238"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>123</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>398933</xdr:colOff>
-      <xdr:row>149</xdr:row>
-      <xdr:rowOff>123190</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Picture 12">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1EB5C29-11F3-C80C-5BBF-B0E927E29474}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="609600" y="23431500"/>
-          <a:ext cx="8933333" cy="5076190"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
       <xdr:row>151</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -448,7 +373,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -492,7 +417,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -501,6 +426,319 @@
         <a:xfrm>
           <a:off x="609600" y="32575500"/>
           <a:ext cx="9152381" cy="6085714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>123</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>149</xdr:row>
+      <xdr:rowOff>181415</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C0988DD-21A0-C489-CB53-5F61C0937E87}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="23431501"/>
+          <a:ext cx="8905875" cy="5134414"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>494171</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>47000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E36FF00-1607-C415-126F-31DCC6CD46BD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="14287500"/>
+          <a:ext cx="9028571" cy="5000000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>103619</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>123476</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B2CA013-9036-4795-0E88-35C1A83CA189}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="381000"/>
+          <a:ext cx="9247619" cy="2790476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>346605</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>171451</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{044E24BF-D342-2419-125F-2C00CD3EA344}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="8001001"/>
+          <a:ext cx="10709805" cy="5695950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>93034</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{785F298B-383A-2F1A-829C-D976CF95D2ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="14097000"/>
+          <a:ext cx="10772775" cy="5236534"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>153061</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01CB83F0-8ABC-0F91-E631-165D44721953}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="19621500"/>
+          <a:ext cx="10877550" cy="5487061"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>160686</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>190000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BA205C0-4DA8-5974-FFC1-C002141EE099}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="3619500"/>
+          <a:ext cx="9914286" cy="4000000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -777,8 +1015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:Q171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
-      <selection activeCell="B205" sqref="B205"/>
+    <sheetView topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="P112" sqref="P112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,22 +1043,22 @@
     </row>
     <row r="111" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P111" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="112" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P112" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="165" spans="1:17" x14ac:dyDescent="0.25">
       <c r="Q165" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="166" spans="1:17" x14ac:dyDescent="0.25">
       <c r="Q166" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="167" spans="1:17" x14ac:dyDescent="0.25">
@@ -831,7 +1069,7 @@
     </row>
     <row r="171" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -839,4 +1077,45 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE35D523-EB92-4092-9F95-CD11EBB8528C}">
+  <dimension ref="A2:B103"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Lấy giá vàng SJC XML
</commit_message>
<xml_diff>
--- a/me-docs/33.Xay-dung-Frontend-hien-thi-tin-tuc-RSS.xlsx
+++ b/me-docs/33.Xay-dung-Frontend-hien-thi-tin-tuc-RSS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\proj_news\me-docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{579B65B1-03DF-4822-8701-ED8EDE85BDE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C4A9874-7FF7-48BC-ACFE-F0D3F659C74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Đọc RSS VNExpress and TuoiTre" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>routes\web.php</t>
   </si>
@@ -62,6 +62,12 @@
   </si>
   <si>
     <t>Result</t>
+  </si>
+  <si>
+    <t>data đọc được là 1 đối tượng SimpleXMLElement</t>
+  </si>
+  <si>
+    <t>dùng json_encode và json_decode để chuyển về mảng</t>
   </si>
 </sst>
 </file>
@@ -711,17 +717,17 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>160686</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>427505</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>190000</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BA205C0-4DA8-5974-FFC1-C002141EE099}"/>
+      <xdr:rowOff>180476</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CF0E087-2B75-2FBA-A26B-45B9644FFA64}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -738,7 +744,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="609600" y="3619500"/>
-          <a:ext cx="9914286" cy="4000000"/>
+          <a:ext cx="8961905" cy="3990476"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1015,8 +1021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:Q171"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="P112" sqref="P112"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="R87" sqref="R87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,6 +1045,16 @@
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q81" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="82" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q82" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="111" spans="16:16" x14ac:dyDescent="0.25">
@@ -1083,7 +1099,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE35D523-EB92-4092-9F95-CD11EBB8528C}">
   <dimension ref="A2:B103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>

</xml_diff>